<commit_message>
Atualização automática de MARAU.xlsx
</commit_message>
<xml_diff>
--- a/MARAU.xlsx
+++ b/MARAU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7075A803-C23C-4CB9-A5A0-B43318718A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{40DFB582-D758-4BCD-96F4-BF8AD32521FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,20 +23,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="7" r:id="rId8"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1333,7 +1320,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1394,30 +1381,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1435,7 +1398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1474,17 +1437,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1531,7 +1489,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{30AAE204-C4E4-4FC5-AD4A-46C4D29ADE38}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{899FA617-A057-45BD-BC5A-E02BB272958E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1561,10 +1519,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08D652E0-D55E-4F84-AAEA-E4956E0AF3EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{204B6896-E3D1-414A-8C75-643EFB7D9D3B}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1602,7 +1560,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1882DC2-239D-4E99-9E88-A09577F99360}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4623E77-97FF-447B-8DCB-8A6BA73CA316}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1665,7 +1623,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49283997-C7E1-46EB-91C9-5231FF05A9E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E6E181A-F384-4CC1-B697-99D92AF06D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1684,7 +1642,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B7AF323-05F3-8CD5-12FE-79B86C14454B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53937666-20C6-5D96-A1B7-38309F5E0A64}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1733,7 +1691,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98699202-9697-BC3A-E721-7504EAA9A219}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF9F2071-4FA7-1895-4C6D-BA21C92910CF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1752,7 +1710,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E784F61D-F661-1DD8-52E1-DA24FDD956D6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AA97061-79D7-59FA-E7DC-68E09D3446CB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1783,7 +1741,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9A7C61B-F605-344D-3015-476D1F5ED17E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7037DDCB-C87A-6E11-5D33-4D7600AF6DD0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1814,7 +1772,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF647638-3F39-B737-F4FE-77699D5B9089}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6C07E3B-68A0-B5B7-98DA-C0355C24F153}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1857,7 +1815,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF6B2312-4929-426E-829A-308E9F804DCB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C78EDEB-C2C6-416D-AE4E-1514388C9C51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1895,7 +1853,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A17DEDA-E687-4511-88FC-9AC915A7CDB1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23537728-11C4-414D-BD39-1CC66F3D7C7E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1938,7 +1896,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{998A5F0B-05DF-47A6-AD77-D1324CEC0D36}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5183FDBA-09E0-4AB6-AE04-FE3AB96D7C5E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2251,7 +2209,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D02058-EF95-4688-AB8B-C73F19177C08}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5342C57E-43C5-4556-953C-27D7DF934832}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2263,98 +2221,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="41"/>
-    <col min="6" max="6" width="2" style="41" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="41" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="41"/>
+    <col min="1" max="5" width="12.5703125" style="38"/>
+    <col min="6" max="6" width="2" style="38" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="38" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="40"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="40"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="40"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="40"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="40"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="40"/>
+      <c r="F6" s="37"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="40"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="40"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="40"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="40"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="40"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="40"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="40"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="40"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="40"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="40"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="40"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="40"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="40"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="40"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="40"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="40"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="40"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="40"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="40"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="40"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="40"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="40"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="40"/>
+      <c r="F29" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5616,19 +5574,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>272</v>
       </c>
     </row>
@@ -5662,46 +5620,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="17" t="s">
         <v>283</v>
       </c>
     </row>
@@ -5709,7 +5667,7 @@
       <c r="A2" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="19">
         <v>44184</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5721,10 +5679,10 @@
       <c r="E2" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="20">
         <v>74.8</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="20">
         <v>748</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -5753,7 +5711,7 @@
       <c r="A3" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="19">
         <v>53160</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5765,10 +5723,10 @@
       <c r="E3" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <v>31.04</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="20">
         <v>310.39999999999998</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -5797,7 +5755,7 @@
       <c r="A4" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="19">
         <v>62177</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -5809,10 +5767,10 @@
       <c r="E4" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="20">
         <v>21.5</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="20">
         <v>214.95</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -5841,7 +5799,7 @@
       <c r="A5" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="19">
         <v>64840</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -5853,10 +5811,10 @@
       <c r="E5" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="20">
         <v>85.8</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="20">
         <v>858</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -5885,7 +5843,7 @@
       <c r="A6" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="19">
         <v>110947</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5897,10 +5855,10 @@
       <c r="E6" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="20">
         <v>32</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="20">
         <v>320</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -5929,7 +5887,7 @@
       <c r="A7" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="19">
         <v>110973</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -5941,10 +5899,10 @@
       <c r="E7" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="20">
         <v>32</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="20">
         <v>320</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -5973,7 +5931,7 @@
       <c r="A8" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="19">
         <v>110975</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -5985,10 +5943,10 @@
       <c r="E8" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="20">
         <v>32</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="20">
         <v>320</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -6017,7 +5975,7 @@
       <c r="A9" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="19">
         <v>110990</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -6029,10 +5987,10 @@
       <c r="E9" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="20">
         <v>32</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="20">
         <v>320</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -6061,7 +6019,7 @@
       <c r="A10" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="19">
         <v>115727</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -6073,10 +6031,10 @@
       <c r="E10" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="20">
         <v>19.899999999999999</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="20">
         <v>199</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -6105,7 +6063,7 @@
       <c r="A11" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="19">
         <v>168614</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -6117,10 +6075,10 @@
       <c r="E11" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="20">
         <v>64.8</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="20">
         <v>648</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -6149,7 +6107,7 @@
       <c r="A12" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="19">
         <v>241343</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -6161,10 +6119,10 @@
       <c r="E12" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="20">
         <v>22.4</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="20">
         <v>224</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -6193,7 +6151,7 @@
       <c r="A13" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="19">
         <v>241396</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -6205,10 +6163,10 @@
       <c r="E13" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="20">
         <v>20.6</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="20">
         <v>206</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -6237,7 +6195,7 @@
       <c r="A14" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="19">
         <v>259450</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -6249,10 +6207,10 @@
       <c r="E14" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="20">
         <v>18.5</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="20">
         <v>185</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -6281,7 +6239,7 @@
       <c r="A15" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="19">
         <v>259451</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -6293,10 +6251,10 @@
       <c r="E15" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="20">
         <v>18.5</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="20">
         <v>185</v>
       </c>
       <c r="H15" s="2" t="s">
@@ -6325,7 +6283,7 @@
       <c r="A16" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="19">
         <v>276786</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -6337,10 +6295,10 @@
       <c r="E16" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="20">
         <v>24.39</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="20">
         <v>243.89</v>
       </c>
       <c r="H16" s="2" t="s">
@@ -6369,7 +6327,7 @@
       <c r="A17" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="19">
         <v>276791</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -6381,10 +6339,10 @@
       <c r="E17" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="20">
         <v>24.39</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="20">
         <v>243.89</v>
       </c>
       <c r="H17" s="2" t="s">
@@ -6413,7 +6371,7 @@
       <c r="A18" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="19">
         <v>276794</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -6425,10 +6383,10 @@
       <c r="E18" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="20">
         <v>24.39</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="20">
         <v>243.89</v>
       </c>
       <c r="H18" s="2" t="s">
@@ -6457,7 +6415,7 @@
       <c r="A19" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="19">
         <v>276801</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -6469,10 +6427,10 @@
       <c r="E19" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="20">
         <v>24.39</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="20">
         <v>243.89</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -6501,7 +6459,7 @@
       <c r="A20" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="19">
         <v>276803</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -6513,10 +6471,10 @@
       <c r="E20" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="20">
         <v>24.39</v>
       </c>
-      <c r="G20" s="23">
+      <c r="G20" s="20">
         <v>243.89</v>
       </c>
       <c r="H20" s="2" t="s">
@@ -6545,7 +6503,7 @@
       <c r="A21" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="19">
         <v>276807</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -6557,10 +6515,10 @@
       <c r="E21" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="20">
         <v>24.39</v>
       </c>
-      <c r="G21" s="23">
+      <c r="G21" s="20">
         <v>243.89</v>
       </c>
       <c r="H21" s="2" t="s">
@@ -6589,7 +6547,7 @@
       <c r="A22" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="19">
         <v>276811</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -6601,10 +6559,10 @@
       <c r="E22" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="20">
         <v>24.39</v>
       </c>
-      <c r="G22" s="23">
+      <c r="G22" s="20">
         <v>243.89</v>
       </c>
       <c r="H22" s="2" t="s">
@@ -6633,7 +6591,7 @@
       <c r="A23" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="19">
         <v>276812</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -6645,10 +6603,10 @@
       <c r="E23" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F23" s="23">
+      <c r="F23" s="20">
         <v>24.39</v>
       </c>
-      <c r="G23" s="23">
+      <c r="G23" s="20">
         <v>243.89</v>
       </c>
       <c r="H23" s="2" t="s">
@@ -6677,7 +6635,7 @@
       <c r="A24" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B24" s="22">
+      <c r="B24" s="19">
         <v>276813</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -6689,10 +6647,10 @@
       <c r="E24" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="20">
         <v>24.39</v>
       </c>
-      <c r="G24" s="23">
+      <c r="G24" s="20">
         <v>243.89</v>
       </c>
       <c r="H24" s="2" t="s">
@@ -6721,7 +6679,7 @@
       <c r="A25" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B25" s="19">
         <v>300101</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -6733,10 +6691,10 @@
       <c r="E25" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="20">
         <v>23.8</v>
       </c>
-      <c r="G25" s="23">
+      <c r="G25" s="20">
         <v>238</v>
       </c>
       <c r="H25" s="2" t="s">
@@ -6765,7 +6723,7 @@
       <c r="A26" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B26" s="22">
+      <c r="B26" s="19">
         <v>300102</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -6777,10 +6735,10 @@
       <c r="E26" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="20">
         <v>23.8</v>
       </c>
-      <c r="G26" s="23">
+      <c r="G26" s="20">
         <v>238</v>
       </c>
       <c r="H26" s="2" t="s">
@@ -6809,7 +6767,7 @@
       <c r="A27" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B27" s="22">
+      <c r="B27" s="19">
         <v>316364</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -6821,10 +6779,10 @@
       <c r="E27" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="20">
         <v>22.48</v>
       </c>
-      <c r="G27" s="23">
+      <c r="G27" s="20">
         <v>224.8</v>
       </c>
       <c r="H27" s="2" t="s">
@@ -6853,7 +6811,7 @@
       <c r="A28" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B28" s="22">
+      <c r="B28" s="19">
         <v>327412</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -6865,10 +6823,10 @@
       <c r="E28" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="20">
         <v>22.48</v>
       </c>
-      <c r="G28" s="23">
+      <c r="G28" s="20">
         <v>224.8</v>
       </c>
       <c r="H28" s="2" t="s">
@@ -6897,7 +6855,7 @@
       <c r="A29" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B29" s="22">
+      <c r="B29" s="19">
         <v>327413</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -6909,10 +6867,10 @@
       <c r="E29" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F29" s="23">
+      <c r="F29" s="20">
         <v>22.48</v>
       </c>
-      <c r="G29" s="23">
+      <c r="G29" s="20">
         <v>224.8</v>
       </c>
       <c r="H29" s="2" t="s">
@@ -6941,7 +6899,7 @@
       <c r="A30" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B30" s="22">
+      <c r="B30" s="19">
         <v>327423</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -6953,10 +6911,10 @@
       <c r="E30" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F30" s="23">
+      <c r="F30" s="20">
         <v>22.48</v>
       </c>
-      <c r="G30" s="23">
+      <c r="G30" s="20">
         <v>224.8</v>
       </c>
       <c r="H30" s="2" t="s">
@@ -6985,7 +6943,7 @@
       <c r="A31" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B31" s="22">
+      <c r="B31" s="19">
         <v>327424</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -6997,10 +6955,10 @@
       <c r="E31" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F31" s="23">
+      <c r="F31" s="20">
         <v>22.48</v>
       </c>
-      <c r="G31" s="23">
+      <c r="G31" s="20">
         <v>224.8</v>
       </c>
       <c r="H31" s="2" t="s">
@@ -7029,7 +6987,7 @@
       <c r="A32" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B32" s="22">
+      <c r="B32" s="19">
         <v>327426</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -7041,10 +6999,10 @@
       <c r="E32" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="20">
         <v>22.48</v>
       </c>
-      <c r="G32" s="23">
+      <c r="G32" s="20">
         <v>224.8</v>
       </c>
       <c r="H32" s="2" t="s">
@@ -7073,7 +7031,7 @@
       <c r="A33" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B33" s="22">
+      <c r="B33" s="19">
         <v>327427</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -7085,10 +7043,10 @@
       <c r="E33" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F33" s="23">
+      <c r="F33" s="20">
         <v>22.48</v>
       </c>
-      <c r="G33" s="23">
+      <c r="G33" s="20">
         <v>224.8</v>
       </c>
       <c r="H33" s="2" t="s">
@@ -7117,7 +7075,7 @@
       <c r="A34" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B34" s="22">
+      <c r="B34" s="19">
         <v>327429</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -7129,10 +7087,10 @@
       <c r="E34" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="20">
         <v>22.48</v>
       </c>
-      <c r="G34" s="23">
+      <c r="G34" s="20">
         <v>224.8</v>
       </c>
       <c r="H34" s="2" t="s">
@@ -7161,7 +7119,7 @@
       <c r="A35" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B35" s="22">
+      <c r="B35" s="19">
         <v>327430</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -7173,10 +7131,10 @@
       <c r="E35" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="20">
         <v>22.48</v>
       </c>
-      <c r="G35" s="23">
+      <c r="G35" s="20">
         <v>224.8</v>
       </c>
       <c r="H35" s="2" t="s">
@@ -7205,7 +7163,7 @@
       <c r="A36" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B36" s="22">
+      <c r="B36" s="19">
         <v>329608</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -7217,10 +7175,10 @@
       <c r="E36" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="20">
         <v>34.5</v>
       </c>
-      <c r="G36" s="23">
+      <c r="G36" s="20">
         <v>345</v>
       </c>
       <c r="H36" s="2" t="s">
@@ -7249,7 +7207,7 @@
       <c r="A37" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B37" s="22">
+      <c r="B37" s="19">
         <v>337196</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -7261,10 +7219,10 @@
       <c r="E37" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F37" s="20">
         <v>34.5</v>
       </c>
-      <c r="G37" s="23">
+      <c r="G37" s="20">
         <v>345</v>
       </c>
       <c r="H37" s="2" t="s">
@@ -7293,7 +7251,7 @@
       <c r="A38" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B38" s="22">
+      <c r="B38" s="19">
         <v>337237</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -7305,10 +7263,10 @@
       <c r="E38" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F38" s="23">
+      <c r="F38" s="20">
         <v>34.5</v>
       </c>
-      <c r="G38" s="23">
+      <c r="G38" s="20">
         <v>345</v>
       </c>
       <c r="H38" s="2" t="s">
@@ -7337,7 +7295,7 @@
       <c r="A39" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B39" s="22">
+      <c r="B39" s="19">
         <v>337238</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -7349,10 +7307,10 @@
       <c r="E39" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F39" s="23">
+      <c r="F39" s="20">
         <v>34.5</v>
       </c>
-      <c r="G39" s="23">
+      <c r="G39" s="20">
         <v>345</v>
       </c>
       <c r="H39" s="2" t="s">
@@ -7381,7 +7339,7 @@
       <c r="A40" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B40" s="22">
+      <c r="B40" s="19">
         <v>337239</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -7393,10 +7351,10 @@
       <c r="E40" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F40" s="20">
         <v>34.5</v>
       </c>
-      <c r="G40" s="23">
+      <c r="G40" s="20">
         <v>345</v>
       </c>
       <c r="H40" s="2" t="s">
@@ -7425,7 +7383,7 @@
       <c r="A41" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B41" s="22">
+      <c r="B41" s="19">
         <v>337240</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -7437,10 +7395,10 @@
       <c r="E41" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F41" s="23">
+      <c r="F41" s="20">
         <v>34.5</v>
       </c>
-      <c r="G41" s="23">
+      <c r="G41" s="20">
         <v>345</v>
       </c>
       <c r="H41" s="2" t="s">
@@ -7469,7 +7427,7 @@
       <c r="A42" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B42" s="22">
+      <c r="B42" s="19">
         <v>337242</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -7481,10 +7439,10 @@
       <c r="E42" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F42" s="23">
+      <c r="F42" s="20">
         <v>34.5</v>
       </c>
-      <c r="G42" s="23">
+      <c r="G42" s="20">
         <v>345</v>
       </c>
       <c r="H42" s="2" t="s">
@@ -7513,7 +7471,7 @@
       <c r="A43" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B43" s="22">
+      <c r="B43" s="19">
         <v>334768</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -7525,10 +7483,10 @@
       <c r="E43" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F43" s="23">
+      <c r="F43" s="20">
         <v>34.5</v>
       </c>
-      <c r="G43" s="23">
+      <c r="G43" s="20">
         <v>345</v>
       </c>
       <c r="H43" s="2" t="s">
@@ -7557,7 +7515,7 @@
       <c r="A44" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B44" s="22">
+      <c r="B44" s="19">
         <v>336059</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -7569,10 +7527,10 @@
       <c r="E44" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F44" s="23">
+      <c r="F44" s="20">
         <v>34.5</v>
       </c>
-      <c r="G44" s="23">
+      <c r="G44" s="20">
         <v>345</v>
       </c>
       <c r="H44" s="2" t="s">
@@ -7601,7 +7559,7 @@
       <c r="A45" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B45" s="22">
+      <c r="B45" s="19">
         <v>336072</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -7613,10 +7571,10 @@
       <c r="E45" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F45" s="23">
+      <c r="F45" s="20">
         <v>34.5</v>
       </c>
-      <c r="G45" s="23">
+      <c r="G45" s="20">
         <v>345</v>
       </c>
       <c r="H45" s="2" t="s">
@@ -7645,7 +7603,7 @@
       <c r="A46" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B46" s="22">
+      <c r="B46" s="19">
         <v>336078</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -7657,10 +7615,10 @@
       <c r="E46" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F46" s="23">
+      <c r="F46" s="20">
         <v>34.5</v>
       </c>
-      <c r="G46" s="23">
+      <c r="G46" s="20">
         <v>345</v>
       </c>
       <c r="H46" s="2" t="s">
@@ -7689,7 +7647,7 @@
       <c r="A47" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B47" s="22">
+      <c r="B47" s="19">
         <v>352087</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -7701,10 +7659,10 @@
       <c r="E47" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F47" s="23">
+      <c r="F47" s="20">
         <v>18.8</v>
       </c>
-      <c r="G47" s="23">
+      <c r="G47" s="20">
         <v>188</v>
       </c>
       <c r="H47" s="2" t="s">
@@ -7733,7 +7691,7 @@
       <c r="A48" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B48" s="22">
+      <c r="B48" s="19">
         <v>349065</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -7745,10 +7703,10 @@
       <c r="E48" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="F48" s="23">
+      <c r="F48" s="20">
         <v>35.200000000000003</v>
       </c>
-      <c r="G48" s="23">
+      <c r="G48" s="20">
         <v>351.99</v>
       </c>
       <c r="H48" s="2" t="s">
@@ -7777,7 +7735,7 @@
       <c r="A49" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B49" s="22">
+      <c r="B49" s="19">
         <v>372618</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -7789,10 +7747,10 @@
       <c r="E49" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="F49" s="23">
+      <c r="F49" s="20">
         <v>30.7</v>
       </c>
-      <c r="G49" s="23">
+      <c r="G49" s="20">
         <v>307</v>
       </c>
       <c r="H49" s="2" t="s">
@@ -7821,7 +7779,7 @@
       <c r="A50" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B50" s="22">
+      <c r="B50" s="19">
         <v>372639</v>
       </c>
       <c r="C50" s="2" t="s">
@@ -7833,10 +7791,10 @@
       <c r="E50" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="F50" s="23">
+      <c r="F50" s="20">
         <v>30.7</v>
       </c>
-      <c r="G50" s="23">
+      <c r="G50" s="20">
         <v>307</v>
       </c>
       <c r="H50" s="2" t="s">
@@ -7865,7 +7823,7 @@
       <c r="A51" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B51" s="22">
+      <c r="B51" s="19">
         <v>392784</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -7877,10 +7835,10 @@
       <c r="E51" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="F51" s="23">
+      <c r="F51" s="20">
         <v>174.09</v>
       </c>
-      <c r="G51" s="23">
+      <c r="G51" s="20">
         <v>1740.92</v>
       </c>
       <c r="H51" s="2" t="s">
@@ -7909,7 +7867,7 @@
       <c r="A52" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B52" s="22">
+      <c r="B52" s="19">
         <v>393599</v>
       </c>
       <c r="C52" s="2" t="s">
@@ -7921,10 +7879,10 @@
       <c r="E52" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="F52" s="23">
+      <c r="F52" s="20">
         <v>33.11</v>
       </c>
-      <c r="G52" s="23">
+      <c r="G52" s="20">
         <v>331.08</v>
       </c>
       <c r="H52" s="2" t="s">
@@ -7953,7 +7911,7 @@
       <c r="A53" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B53" s="22">
+      <c r="B53" s="19">
         <v>398379</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -7965,10 +7923,10 @@
       <c r="E53" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="F53" s="23">
+      <c r="F53" s="20">
         <v>174.09</v>
       </c>
-      <c r="G53" s="23">
+      <c r="G53" s="20">
         <v>1740.92</v>
       </c>
       <c r="H53" s="2" t="s">
@@ -7997,7 +7955,7 @@
       <c r="A54" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B54" s="22">
+      <c r="B54" s="19">
         <v>405263</v>
       </c>
       <c r="C54" s="2" t="s">
@@ -8009,10 +7967,10 @@
       <c r="E54" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F54" s="23">
+      <c r="F54" s="20">
         <v>31.45</v>
       </c>
-      <c r="G54" s="23">
+      <c r="G54" s="20">
         <v>314.47000000000003</v>
       </c>
       <c r="H54" s="2" t="s">
@@ -8041,7 +7999,7 @@
       <c r="A55" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B55" s="22">
+      <c r="B55" s="19">
         <v>413111</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -8053,10 +8011,10 @@
       <c r="E55" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F55" s="23">
+      <c r="F55" s="20">
         <v>31.45</v>
       </c>
-      <c r="G55" s="23">
+      <c r="G55" s="20">
         <v>314.47000000000003</v>
       </c>
       <c r="H55" s="2" t="s">
@@ -8085,7 +8043,7 @@
       <c r="A56" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B56" s="22">
+      <c r="B56" s="19">
         <v>437239</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -8097,10 +8055,10 @@
       <c r="E56" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="F56" s="23">
+      <c r="F56" s="20">
         <v>36.53</v>
       </c>
-      <c r="G56" s="23">
+      <c r="G56" s="20">
         <v>365.25</v>
       </c>
       <c r="H56" s="2" t="s">
@@ -8129,7 +8087,7 @@
       <c r="A57" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B57" s="22">
+      <c r="B57" s="19">
         <v>437758</v>
       </c>
       <c r="C57" s="2" t="s">
@@ -8141,10 +8099,10 @@
       <c r="E57" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="F57" s="23">
+      <c r="F57" s="20">
         <v>36.53</v>
       </c>
-      <c r="G57" s="23">
+      <c r="G57" s="20">
         <v>365.25</v>
       </c>
       <c r="H57" s="2" t="s">
@@ -8173,7 +8131,7 @@
       <c r="A58" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B58" s="22">
+      <c r="B58" s="19">
         <v>437759</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -8185,10 +8143,10 @@
       <c r="E58" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="F58" s="23">
+      <c r="F58" s="20">
         <v>36.53</v>
       </c>
-      <c r="G58" s="23">
+      <c r="G58" s="20">
         <v>365.25</v>
       </c>
       <c r="H58" s="2" t="s">
@@ -8217,7 +8175,7 @@
       <c r="A59" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B59" s="22">
+      <c r="B59" s="19">
         <v>437988</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -8229,10 +8187,10 @@
       <c r="E59" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="F59" s="23">
+      <c r="F59" s="20">
         <v>1661.52</v>
       </c>
-      <c r="G59" s="23">
+      <c r="G59" s="20">
         <v>3864</v>
       </c>
       <c r="H59" s="2" t="s">
@@ -8261,7 +8219,7 @@
       <c r="A60" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B60" s="22">
+      <c r="B60" s="19">
         <v>453692</v>
       </c>
       <c r="C60" s="2" t="s">
@@ -8273,10 +8231,10 @@
       <c r="E60" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="F60" s="23">
+      <c r="F60" s="20">
         <v>4007.15</v>
       </c>
-      <c r="G60" s="23">
+      <c r="G60" s="20">
         <v>7490</v>
       </c>
       <c r="H60" s="2" t="s">
@@ -8305,7 +8263,7 @@
       <c r="A61" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B61" s="22">
+      <c r="B61" s="19">
         <v>453693</v>
       </c>
       <c r="C61" s="2" t="s">
@@ -8317,10 +8275,10 @@
       <c r="E61" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="F61" s="23">
+      <c r="F61" s="20">
         <v>2874.02</v>
       </c>
-      <c r="G61" s="23">
+      <c r="G61" s="20">
         <v>5372</v>
       </c>
       <c r="H61" s="2" t="s">
@@ -8349,7 +8307,7 @@
       <c r="A62" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B62" s="22">
+      <c r="B62" s="19">
         <v>453694</v>
       </c>
       <c r="C62" s="2" t="s">
@@ -8361,10 +8319,10 @@
       <c r="E62" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="F62" s="23">
+      <c r="F62" s="20">
         <v>329.18</v>
       </c>
-      <c r="G62" s="23">
+      <c r="G62" s="20">
         <v>615</v>
       </c>
       <c r="H62" s="2" t="s">
@@ -8393,7 +8351,7 @@
       <c r="A63" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B63" s="22">
+      <c r="B63" s="19">
         <v>453695</v>
       </c>
       <c r="C63" s="2" t="s">
@@ -8405,10 +8363,10 @@
       <c r="E63" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="F63" s="23">
+      <c r="F63" s="20">
         <v>329.18</v>
       </c>
-      <c r="G63" s="23">
+      <c r="G63" s="20">
         <v>615</v>
       </c>
       <c r="H63" s="2" t="s">
@@ -8437,7 +8395,7 @@
       <c r="A64" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B64" s="22">
+      <c r="B64" s="19">
         <v>453696</v>
       </c>
       <c r="C64" s="2" t="s">
@@ -8449,10 +8407,10 @@
       <c r="E64" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="F64" s="23">
+      <c r="F64" s="20">
         <v>663.4</v>
       </c>
-      <c r="G64" s="23">
+      <c r="G64" s="20">
         <v>1240</v>
       </c>
       <c r="H64" s="2" t="s">
@@ -8481,7 +8439,7 @@
       <c r="A65" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B65" s="22">
+      <c r="B65" s="19">
         <v>459315</v>
       </c>
       <c r="C65" s="2" t="s">
@@ -8493,10 +8451,10 @@
       <c r="E65" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="F65" s="23">
+      <c r="F65" s="20">
         <v>566.52</v>
       </c>
-      <c r="G65" s="23">
+      <c r="G65" s="20">
         <v>654.9</v>
       </c>
       <c r="H65" s="2" t="s">
@@ -8525,7 +8483,7 @@
       <c r="A66" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B66" s="22">
+      <c r="B66" s="19">
         <v>459316</v>
       </c>
       <c r="C66" s="2" t="s">
@@ -8537,10 +8495,10 @@
       <c r="E66" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="F66" s="23">
+      <c r="F66" s="20">
         <v>566.52</v>
       </c>
-      <c r="G66" s="23">
+      <c r="G66" s="20">
         <v>654.9</v>
       </c>
       <c r="H66" s="2" t="s">
@@ -8569,7 +8527,7 @@
       <c r="A67" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B67" s="22">
+      <c r="B67" s="19">
         <v>459317</v>
       </c>
       <c r="C67" s="2" t="s">
@@ -8581,10 +8539,10 @@
       <c r="E67" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="F67" s="23">
+      <c r="F67" s="20">
         <v>566.52</v>
       </c>
-      <c r="G67" s="23">
+      <c r="G67" s="20">
         <v>654.9</v>
       </c>
       <c r="H67" s="2" t="s">
@@ -8613,7 +8571,7 @@
       <c r="A68" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B68" s="22">
+      <c r="B68" s="19">
         <v>459318</v>
       </c>
       <c r="C68" s="2" t="s">
@@ -8625,10 +8583,10 @@
       <c r="E68" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="F68" s="23">
+      <c r="F68" s="20">
         <v>566.52</v>
       </c>
-      <c r="G68" s="23">
+      <c r="G68" s="20">
         <v>654.9</v>
       </c>
       <c r="H68" s="2" t="s">
@@ -8657,7 +8615,7 @@
       <c r="A69" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B69" s="22">
+      <c r="B69" s="19">
         <v>459319</v>
       </c>
       <c r="C69" s="2" t="s">
@@ -8669,10 +8627,10 @@
       <c r="E69" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="F69" s="23">
+      <c r="F69" s="20">
         <v>566.52</v>
       </c>
-      <c r="G69" s="23">
+      <c r="G69" s="20">
         <v>654.9</v>
       </c>
       <c r="H69" s="2" t="s">
@@ -8711,14 +8669,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>361</v>
       </c>
     </row>
@@ -8749,46 +8707,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>362</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>364</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="23" t="s">
         <v>367</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="23" t="s">
         <v>365</v>
       </c>
     </row>
@@ -8813,54 +8771,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>368</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>369</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>370</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>371</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>372</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>373</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>374</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>375</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>377</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>378</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>379</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>380</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>381</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="24" t="s">
         <v>382</v>
       </c>
     </row>
@@ -8871,43 +8830,43 @@
       <c r="B2" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="27">
         <v>45078</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="28">
         <v>3930</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="28" t="s">
         <v>384</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="29">
         <v>11384</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="29">
         <v>1239</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="30" t="s">
         <v>386</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="30" t="s">
         <v>386</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="30" t="s">
         <v>386</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="30" t="s">
         <v>386</v>
       </c>
-      <c r="M2" s="34" t="s">
+      <c r="M2" s="31" t="s">
         <v>387</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="31" t="s">
         <v>387</v>
       </c>
     </row>
@@ -8938,25 +8897,24 @@
       <c r="B1" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="32" t="s">
         <v>389</v>
       </c>
-      <c r="E1" s="36">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="33">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2" s="36">
         <v>252</v>
       </c>
-      <c r="F1" s="37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="B2" s="39">
-        <v>252</v>
-      </c>
-      <c r="C2" s="37">
+      <c r="C2" s="34">
         <v>1.666446237270202E-2</v>
       </c>
     </row>

</xml_diff>